<commit_message>
Support for each database platform.
</commit_message>
<xml_diff>
--- a/src/test/resources/org/penguinframework/test/dao/expected_all_type.xlsx
+++ b/src/test/resources/org/penguinframework/test/dao/expected_all_type.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\penguinframework-test\src\test\resources\org\penguinframework\test\dao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F0A16DA-5D3A-4869-B567-47E952BCC482}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBAFF8F9-CB33-4266-8D39-A7849EFBF6BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>int_type</t>
   </si>
@@ -105,7 +105,11 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Z3ne+21JTi6z3ZXNBxzqXA==</t>
+    <t>12:13:14.987654321</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>6779defb-6d49-4e2e-b3dd-95cd071cea5c</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -149,11 +153,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -434,7 +439,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -508,62 +513,70 @@
       </c>
     </row>
     <row r="2" spans="1:19">
-      <c r="A2" s="2">
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
+      <c r="A3" s="2">
         <v>123456789</v>
       </c>
-      <c r="B2" s="2" t="b">
+      <c r="B3" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C3" s="2">
         <v>127</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D3" s="2">
         <v>32767</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E3" s="2">
         <v>999999999</v>
       </c>
-      <c r="F2" s="2">
-        <v>1</v>
-      </c>
-      <c r="G2" s="2">
+      <c r="F3" s="2">
+        <v>2</v>
+      </c>
+      <c r="G3" s="2">
         <v>3.1415926535898002</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H3" s="2">
         <v>3.1415920000000002</v>
       </c>
-      <c r="I2" s="2">
+      <c r="I3" s="2">
         <v>3.14</v>
       </c>
-      <c r="J2" s="3">
+      <c r="J3" s="3">
         <v>25569.551562500001</v>
       </c>
-      <c r="K2" s="1">
+      <c r="K3" s="1">
         <v>44530</v>
       </c>
-      <c r="L2" s="3">
+      <c r="L3" s="3">
         <v>44530.551562499997</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="O3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="P3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="Q3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="R3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="S2" s="2" t="s">
-        <v>25</v>
+      <c r="S3" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>